<commit_message>
Changed code leader and discussion dates for student
</commit_message>
<xml_diff>
--- a/Group, Coding Assignment, Leading Discussion/Group, Coding Assignment, Leading Discussion.xlsx
+++ b/Group, Coding Assignment, Leading Discussion/Group, Coding Assignment, Leading Discussion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jared_Edgerton\Dropbox\teaching_material\PSU\soda_501\Group, Coding Assignment, Leading Discussion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9AE9956-429D-4C88-B96D-A473B14069D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFB3245-1BA4-4D9D-8A90-3030206DF0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{EC1FA02E-612C-494A-963C-FE1C97348D14}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{EC1FA02E-612C-494A-963C-FE1C97348D14}"/>
   </bookViews>
   <sheets>
     <sheet name="Group" sheetId="1" r:id="rId1"/>
@@ -466,9 +466,9 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,7 +476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -484,7 +484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -492,7 +492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -500,7 +500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -518,12 +518,12 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -531,12 +531,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -544,15 +544,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -560,7 +557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -568,7 +565,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -576,7 +573,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -584,22 +581,25 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -607,7 +607,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -615,12 +615,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -635,12 +635,12 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -648,12 +648,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -661,7 +661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -669,7 +669,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -677,12 +677,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -690,17 +693,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -708,20 +711,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -729,7 +729,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -737,7 +737,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>

</xml_diff>